<commit_message>
bai tap cylinder point
</commit_message>
<xml_diff>
--- a/Nề nếp.xlsx
+++ b/Nề nếp.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85D9023-E412-4C68-A559-15FAD9601258}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AF0C99-60FD-49E7-B7B2-B85D1C16023C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Phan Ngọc Hiếu</t>
   </si>
@@ -29,15 +29,6 @@
   </si>
   <si>
     <t>Hưng</t>
-  </si>
-  <si>
-    <t>10/03: Xin về sớm
-13/03: Đi trễ</t>
-  </si>
-  <si>
-    <t>Sáng 10/03: Đi trễ
-Chiều 10/03: Về sớm
-13/03: Chưa chuẩn bị bài</t>
   </si>
   <si>
     <t>10/3: xin nghỉ
@@ -50,6 +41,29 @@
     <t>13/03: Chưa soạn bài
 14/03: Nghĩa
 13/03: Xin nghỉ</t>
+  </si>
+  <si>
+    <t>Thiện</t>
+  </si>
+  <si>
+    <t>Xóa nợ</t>
+  </si>
+  <si>
+    <t>10/03: Xin về sớm
+13/03: Đi trễ
+16/03: Đi trễ
+16/03: Xin về sơm</t>
+  </si>
+  <si>
+    <t>Sáng 10/03: Đi trễ
+Chiều 10/03: Về sớm
+13/03: Chưa chuẩn bị bài
+15/03: Đau xin nghỉ
+16/03: Đau xin nghỉ</t>
+  </si>
+  <si>
+    <t>16/03: Đi trể
+17/03: Xin nghỉ 1 ngày</t>
   </si>
 </sst>
 </file>
@@ -370,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,36 +397,49 @@
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>